<commit_message>
brought up comp bot, added mirrored paths to automodes
</commit_message>
<xml_diff>
--- a/docs/motormapping.xlsx
+++ b/docs/motormapping.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\butch\robottools\robots\1425\2024\allegro2024\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FB6B4E1-8B45-4CD2-9622-BD8DB59C3795}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C1646C0-EABD-4CC3-B56D-D216AAE7D628}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="20928" windowHeight="12432" xr2:uid="{88448273-EBF9-4EFF-B776-4CCA91CC2981}"/>
   </bookViews>
@@ -501,7 +501,7 @@
   <dimension ref="B13:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -617,14 +617,14 @@
         <v>0</v>
       </c>
       <c r="D20">
-        <v>53.33</v>
+        <v>66</v>
       </c>
       <c r="E20" t="s">
         <v>7</v>
       </c>
       <c r="F20">
         <f>D20*2048</f>
-        <v>109219.84</v>
+        <v>135168</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.55000000000000004">
@@ -642,7 +642,7 @@
       </c>
       <c r="G21">
         <f>F21/F20</f>
-        <v>3.2961044440277519E-3</v>
+        <v>2.6633522727272725E-3</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.55000000000000004">

</xml_diff>

<commit_message>
added alternative start collect approach, updated the gear ratios for the comp bot, added velocity checking to the auto shoot action, changed to target tracker triangle method data from inches to meters
</commit_message>
<xml_diff>
--- a/docs/motormapping.xlsx
+++ b/docs/motormapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\butch\robottools\robots\1425\2024\allegro2024\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C1646C0-EABD-4CC3-B56D-D216AAE7D628}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DB86EBD-126C-416F-B7CD-C9D92FA58944}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="20928" windowHeight="12432" xr2:uid="{88448273-EBF9-4EFF-B776-4CCA91CC2981}"/>
+    <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{88448273-EBF9-4EFF-B776-4CCA91CC2981}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -501,7 +501,7 @@
   <dimension ref="B13:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -653,14 +653,14 @@
         <v>0</v>
       </c>
       <c r="D23">
-        <v>101.56</v>
+        <v>250</v>
       </c>
       <c r="E23" t="s">
         <v>7</v>
       </c>
       <c r="F23">
         <f>D23*2048</f>
-        <v>207994.88</v>
+        <v>512000</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.55000000000000004">
@@ -679,7 +679,7 @@
       </c>
       <c r="G24" s="1">
         <f>F24/F23</f>
-        <v>6.6119416016394249E-7</v>
+        <v>2.6860351562499999E-7</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.55000000000000004">
@@ -690,14 +690,14 @@
         <v>0</v>
       </c>
       <c r="D26">
-        <v>40</v>
+        <v>29.33</v>
       </c>
       <c r="E26" t="s">
         <v>7</v>
       </c>
       <c r="F26">
         <f>D26*2048</f>
-        <v>81920</v>
+        <v>60067.839999999997</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.55000000000000004">
@@ -716,7 +716,7 @@
       </c>
       <c r="G27" s="1">
         <f>F27/F26</f>
-        <v>1.3729858398437499E-6</v>
+        <v>1.8724661982185475E-6</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.55000000000000004">
@@ -727,14 +727,14 @@
         <v>0</v>
       </c>
       <c r="D29">
-        <v>12.5</v>
+        <v>14.81</v>
       </c>
       <c r="E29" t="s">
         <v>7</v>
       </c>
       <c r="F29">
         <f>D29*2048</f>
-        <v>25600</v>
+        <v>30330.880000000001</v>
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.55000000000000004">
@@ -752,7 +752,7 @@
       </c>
       <c r="G30">
         <f>F30/F29</f>
-        <v>1.40625E-2</v>
+        <v>1.18690918298447E-2</v>
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.55000000000000004">

</xml_diff>

<commit_message>
updated to complete trap
</commit_message>
<xml_diff>
--- a/docs/motormapping.xlsx
+++ b/docs/motormapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\butch\robottools\robots\1425\2024\allegro2024\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DB86EBD-126C-416F-B7CD-C9D92FA58944}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59986527-1AAE-4D7A-A97F-8ABD1FC62133}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{88448273-EBF9-4EFF-B776-4CCA91CC2981}"/>
+    <workbookView xWindow="6" yWindow="0" windowWidth="20724" windowHeight="12240" xr2:uid="{88448273-EBF9-4EFF-B776-4CCA91CC2981}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -106,13 +106,13 @@
     <t>Subsystem (in)</t>
   </si>
   <si>
-    <t>Meters</t>
-  </si>
-  <si>
     <t>Power</t>
   </si>
   <si>
     <t>Speed</t>
+  </si>
+  <si>
+    <t>Inches</t>
   </si>
 </sst>
 </file>
@@ -500,8 +500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{465FA729-F0E6-4240-BEC4-9EAF3A8EF9BA}">
   <dimension ref="B13:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -671,7 +671,7 @@
         <v>5.5010000000000003</v>
       </c>
       <c r="E24" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F24">
         <f>D24*0.025</f>
@@ -708,7 +708,7 @@
         <v>4.4989999999999997</v>
       </c>
       <c r="E27" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F27">
         <f>D27*0.025</f>
@@ -809,10 +809,10 @@
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
         <v>16</v>
-      </c>
-      <c r="C2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.55000000000000004">

</xml_diff>

<commit_message>
work from last night on shooting and robot updates
</commit_message>
<xml_diff>
--- a/docs/motormapping.xlsx
+++ b/docs/motormapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\butch\robottools\robots\1425\2024\allegro2024\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59986527-1AAE-4D7A-A97F-8ABD1FC62133}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9430920-1034-4A95-B87A-6DE1BE54EC26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6" yWindow="0" windowWidth="20724" windowHeight="12240" xr2:uid="{88448273-EBF9-4EFF-B776-4CCA91CC2981}"/>
+    <workbookView xWindow="60" yWindow="0" windowWidth="20550" windowHeight="12150" xr2:uid="{88448273-EBF9-4EFF-B776-4CCA91CC2981}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -119,9 +119,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0.0000000000000_);_(* \(#,##0.0000000000000\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="179" formatCode="_(* #,##0.00000000000000000_);_(* \(#,##0.00000000000000000\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -160,9 +161,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -500,8 +502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{465FA729-F0E6-4240-BEC4-9EAF3A8EF9BA}">
   <dimension ref="B13:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -512,7 +514,8 @@
     <col min="5" max="5" width="9.41796875" customWidth="1"/>
     <col min="6" max="6" width="12.3125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.26171875" customWidth="1"/>
-    <col min="8" max="9" width="11.68359375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.26171875" customWidth="1"/>
+    <col min="9" max="9" width="11.68359375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="13" spans="2:10" x14ac:dyDescent="0.55000000000000004">
@@ -573,7 +576,7 @@
         <v>3.3333333333333335</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B17" t="s">
         <v>1</v>
       </c>
@@ -591,7 +594,7 @@
         <v>43683.839999999997</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C18" t="s">
         <v>4</v>
       </c>
@@ -609,7 +612,7 @@
         <v>8.2410337552742616E-3</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B20" t="s">
         <v>9</v>
       </c>
@@ -627,7 +630,7 @@
         <v>135168</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C21" t="s">
         <v>4</v>
       </c>
@@ -645,7 +648,7 @@
         <v>2.6633522727272725E-3</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B23" t="s">
         <v>10</v>
       </c>
@@ -663,7 +666,7 @@
         <v>512000</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C24" t="s">
         <v>14</v>
       </c>
@@ -681,8 +684,12 @@
         <f>F24/F23</f>
         <v>2.6860351562499999E-7</v>
       </c>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="H24" s="2">
+        <f>5*G24</f>
+        <v>1.343017578125E-6</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B26" t="s">
         <v>11</v>
       </c>
@@ -700,7 +707,7 @@
         <v>60067.839999999997</v>
       </c>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C27" t="s">
         <v>14</v>
       </c>
@@ -719,7 +726,7 @@
         <v>1.8724661982185475E-6</v>
       </c>
     </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B29" t="s">
         <v>12</v>
       </c>
@@ -737,7 +744,7 @@
         <v>30330.880000000001</v>
       </c>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C30" t="s">
         <v>4</v>
       </c>
@@ -755,7 +762,7 @@
         <v>1.18690918298447E-2</v>
       </c>
     </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B32" t="s">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
updated the tilt gear ratios
</commit_message>
<xml_diff>
--- a/docs/motormapping.xlsx
+++ b/docs/motormapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\butch\robottools\robots\1425\2024\allegro2024\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9430920-1034-4A95-B87A-6DE1BE54EC26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCA18A6E-B21E-4C70-AF9C-4948959CAEEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="0" windowWidth="20550" windowHeight="12150" xr2:uid="{88448273-EBF9-4EFF-B776-4CCA91CC2981}"/>
+    <workbookView xWindow="-28740" yWindow="0" windowWidth="28800" windowHeight="15195" xr2:uid="{88448273-EBF9-4EFF-B776-4CCA91CC2981}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -122,7 +122,7 @@
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0.0000000000000_);_(* \(#,##0.0000000000000\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="179" formatCode="_(* #,##0.00000000000000000_);_(* \(#,##0.00000000000000000\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0.00000000000000000_);_(* \(#,##0.00000000000000000\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -164,7 +164,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -503,22 +503,22 @@
   <dimension ref="B13:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="O25" sqref="O25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="29.1015625" customWidth="1"/>
-    <col min="3" max="3" width="13.1015625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.41796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.41796875" customWidth="1"/>
-    <col min="6" max="6" width="12.3125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.26171875" customWidth="1"/>
-    <col min="8" max="8" width="31.26171875" customWidth="1"/>
-    <col min="9" max="9" width="11.68359375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.08984375" customWidth="1"/>
+    <col min="3" max="3" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.453125" customWidth="1"/>
+    <col min="6" max="6" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.26953125" customWidth="1"/>
+    <col min="8" max="8" width="31.26953125" customWidth="1"/>
+    <col min="9" max="9" width="11.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
       <c r="C13" t="s">
         <v>3</v>
       </c>
@@ -533,7 +533,7 @@
         <v>1.6666666666666667</v>
       </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>2</v>
       </c>
@@ -551,7 +551,7 @@
         <v>1228.8</v>
       </c>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
       <c r="C15" t="s">
         <v>4</v>
       </c>
@@ -576,7 +576,7 @@
         <v>3.3333333333333335</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
         <v>1</v>
       </c>
@@ -584,17 +584,20 @@
         <v>0</v>
       </c>
       <c r="D17">
-        <v>21.33</v>
+        <v>22.068965517241399</v>
       </c>
       <c r="E17" t="s">
         <v>7</v>
       </c>
       <c r="F17">
         <f>D17*2048</f>
-        <v>43683.839999999997</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+        <v>45197.241379310384</v>
+      </c>
+      <c r="I17">
+        <v>21.33</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.35">
       <c r="C18" t="s">
         <v>4</v>
       </c>
@@ -609,10 +612,10 @@
       </c>
       <c r="G18">
         <f>F18/F17</f>
-        <v>8.2410337552742616E-3</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+        <v>7.9650878906249931E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
         <v>9</v>
       </c>
@@ -630,7 +633,7 @@
         <v>135168</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.35">
       <c r="C21" t="s">
         <v>4</v>
       </c>
@@ -648,7 +651,7 @@
         <v>2.6633522727272725E-3</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
         <v>10</v>
       </c>
@@ -666,7 +669,7 @@
         <v>512000</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.35">
       <c r="C24" t="s">
         <v>14</v>
       </c>
@@ -689,7 +692,7 @@
         <v>1.343017578125E-6</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>11</v>
       </c>
@@ -707,7 +710,7 @@
         <v>60067.839999999997</v>
       </c>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.35">
       <c r="C27" t="s">
         <v>14</v>
       </c>
@@ -726,7 +729,7 @@
         <v>1.8724661982185475E-6</v>
       </c>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
         <v>12</v>
       </c>
@@ -744,7 +747,7 @@
         <v>30330.880000000001</v>
       </c>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.35">
       <c r="C30" t="s">
         <v>4</v>
       </c>
@@ -762,7 +765,7 @@
         <v>1.18690918298447E-2</v>
       </c>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
         <v>13</v>
       </c>
@@ -780,7 +783,7 @@
         <v>2048</v>
       </c>
     </row>
-    <row r="33" spans="3:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C33" t="s">
         <v>4</v>
       </c>
@@ -812,9 +815,9 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>15</v>
       </c>
@@ -822,7 +825,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B3">
         <v>0</v>
       </c>
@@ -830,7 +833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B4">
         <v>0.3</v>
       </c>
@@ -838,7 +841,7 @@
         <v>8.3000000000000004E-2</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B6" cm="1">
         <f t="array" ref="B6:C6">LINEST(C3:C4,B3:B4,FALSE, FALSE)</f>
         <v>0.27666666666666667</v>
@@ -847,7 +850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B8">
         <f>1/B6</f>
         <v>3.6144578313253013</v>

</xml_diff>

<commit_message>
work on the robot 3/29
</commit_message>
<xml_diff>
--- a/docs/motormapping.xlsx
+++ b/docs/motormapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\butch\robottools\robots\1425\2024\allegro2024\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCA18A6E-B21E-4C70-AF9C-4948959CAEEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47A525EC-0368-48C3-A876-F36F6F027227}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28740" yWindow="0" windowWidth="28800" windowHeight="15195" xr2:uid="{88448273-EBF9-4EFF-B776-4CCA91CC2981}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="20928" windowHeight="12432" xr2:uid="{88448273-EBF9-4EFF-B776-4CCA91CC2981}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -500,25 +500,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{465FA729-F0E6-4240-BEC4-9EAF3A8EF9BA}">
-  <dimension ref="B13:J33"/>
+  <dimension ref="B13:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="O25" sqref="O25"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="29.08984375" customWidth="1"/>
-    <col min="3" max="3" width="13.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.453125" customWidth="1"/>
-    <col min="6" max="6" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.26953125" customWidth="1"/>
-    <col min="8" max="8" width="31.26953125" customWidth="1"/>
-    <col min="9" max="9" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.1015625" customWidth="1"/>
+    <col min="3" max="3" width="13.1015625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.47265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.47265625" customWidth="1"/>
+    <col min="6" max="6" width="12.26171875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.26171875" customWidth="1"/>
+    <col min="8" max="8" width="9.20703125" customWidth="1"/>
+    <col min="9" max="9" width="11.62890625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.55000000000000004">
       <c r="C13" t="s">
         <v>3</v>
       </c>
@@ -528,12 +528,8 @@
       <c r="G13" t="s">
         <v>6</v>
       </c>
-      <c r="J13">
-        <f>1/0.6</f>
-        <v>1.6666666666666667</v>
-      </c>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.55000000000000004">
       <c r="B14" t="s">
         <v>2</v>
       </c>
@@ -551,7 +547,7 @@
         <v>1228.8</v>
       </c>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.55000000000000004">
       <c r="C15" t="s">
         <v>4</v>
       </c>
@@ -568,15 +564,8 @@
         <f>F15/F14</f>
         <v>8.1380208333333337E-4</v>
       </c>
-      <c r="I15">
-        <v>2</v>
-      </c>
-      <c r="J15">
-        <f>I15*J13</f>
-        <v>3.3333333333333335</v>
-      </c>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B17" t="s">
         <v>1</v>
       </c>
@@ -584,20 +573,20 @@
         <v>0</v>
       </c>
       <c r="D17">
-        <v>22.068965517241399</v>
+        <v>18</v>
       </c>
       <c r="E17" t="s">
         <v>7</v>
       </c>
       <c r="F17">
         <f>D17*2048</f>
-        <v>45197.241379310384</v>
+        <v>36864</v>
       </c>
       <c r="I17">
-        <v>21.33</v>
-      </c>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.35">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="C18" t="s">
         <v>4</v>
       </c>
@@ -612,10 +601,19 @@
       </c>
       <c r="G18">
         <f>F18/F17</f>
-        <v>7.9650878906249931E-3</v>
-      </c>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.35">
+        <v>9.765625E-3</v>
+      </c>
+      <c r="I18">
+        <v>27.5</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="I19">
+        <f>I18/I17</f>
+        <v>0.41666666666666669</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B20" t="s">
         <v>9</v>
       </c>
@@ -623,17 +621,20 @@
         <v>0</v>
       </c>
       <c r="D20">
-        <v>66</v>
+        <v>49.5</v>
       </c>
       <c r="E20" t="s">
         <v>7</v>
       </c>
       <c r="F20">
         <f>D20*2048</f>
-        <v>135168</v>
-      </c>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.35">
+        <v>101376</v>
+      </c>
+      <c r="I20">
+        <v>5.6000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="C21" t="s">
         <v>4</v>
       </c>
@@ -648,10 +649,14 @@
       </c>
       <c r="G21">
         <f>F21/F20</f>
-        <v>2.6633522727272725E-3</v>
-      </c>
-    </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.35">
+        <v>3.5511363636363635E-3</v>
+      </c>
+      <c r="I21">
+        <f>I19*I20</f>
+        <v>2.3333333333333334E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B23" t="s">
         <v>10</v>
       </c>
@@ -669,7 +674,7 @@
         <v>512000</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="C24" t="s">
         <v>14</v>
       </c>
@@ -687,12 +692,9 @@
         <f>F24/F23</f>
         <v>2.6860351562499999E-7</v>
       </c>
-      <c r="H24" s="2">
-        <f>5*G24</f>
-        <v>1.343017578125E-6</v>
-      </c>
-    </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="H24" s="2"/>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B26" t="s">
         <v>11</v>
       </c>
@@ -710,7 +712,7 @@
         <v>60067.839999999997</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="C27" t="s">
         <v>14</v>
       </c>
@@ -729,7 +731,7 @@
         <v>1.8724661982185475E-6</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B29" t="s">
         <v>12</v>
       </c>
@@ -747,7 +749,7 @@
         <v>30330.880000000001</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="C30" t="s">
         <v>4</v>
       </c>
@@ -765,7 +767,7 @@
         <v>1.18690918298447E-2</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B32" t="s">
         <v>13</v>
       </c>
@@ -783,7 +785,7 @@
         <v>2048</v>
       </c>
     </row>
-    <row r="33" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="3:7" x14ac:dyDescent="0.55000000000000004">
       <c r="C33" t="s">
         <v>4</v>
       </c>
@@ -815,9 +817,9 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" t="s">
         <v>15</v>
       </c>
@@ -825,7 +827,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B3">
         <v>0</v>
       </c>
@@ -833,7 +835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B4">
         <v>0.3</v>
       </c>
@@ -841,7 +843,7 @@
         <v>8.3000000000000004E-2</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B6" cm="1">
         <f t="array" ref="B6:C6">LINEST(C3:C4,B3:B4,FALSE, FALSE)</f>
         <v>0.27666666666666667</v>
@@ -850,7 +852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B8">
         <f>1/B6</f>
         <v>3.6144578313253013</v>

</xml_diff>